<commit_message>
Create Data Provider Add raports Add screenshots to raports
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -22,10 +22,13 @@
     <t>Dubai</t>
   </si>
   <si>
-    <t>xxx</t>
+    <t>Jumeirah Beach Hotel</t>
   </si>
   <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>Grand Plaza Apartments</t>
   </si>
 </sst>
 </file>
@@ -303,7 +306,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>